<commit_message>
Inicio sesion Admin completado
</commit_message>
<xml_diff>
--- a/Diagrama Gantt Tecnovnetas.xlsx
+++ b/Diagrama Gantt Tecnovnetas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Tecnoventas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED2F9C1-C0F3-4865-B19B-2ED3FAB07DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D81C75C-5595-4467-B45F-34AB5FDBCD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -400,31 +400,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -476,8 +461,23 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -532,15 +532,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>5772</xdr:colOff>
+          <xdr:colOff>6350</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>5773</xdr:rowOff>
+          <xdr:rowOff>6350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>236681</xdr:colOff>
+          <xdr:colOff>234950</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>173181</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -782,7 +782,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -798,212 +798,212 @@
       <c r="D1" s="10"/>
     </row>
     <row r="4" spans="1:48" ht="14" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="35">
+      <c r="C4" s="49"/>
+      <c r="D4" s="30">
         <v>0</v>
       </c>
       <c r="E4" s="6">
         <f>D5+D4</f>
         <v>45078</v>
       </c>
-      <c r="G4" s="27">
+      <c r="G4" s="45">
         <f>G5</f>
         <v>45078</v>
       </c>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="27">
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="45">
         <f>N5</f>
         <v>45085</v>
       </c>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="24"/>
-      <c r="U4" s="27">
+      <c r="O4" s="46"/>
+      <c r="P4" s="46"/>
+      <c r="Q4" s="46"/>
+      <c r="R4" s="46"/>
+      <c r="S4" s="46"/>
+      <c r="T4" s="47"/>
+      <c r="U4" s="45">
         <f>U5</f>
         <v>45092</v>
       </c>
-      <c r="V4" s="23"/>
-      <c r="W4" s="23"/>
-      <c r="X4" s="23"/>
-      <c r="Y4" s="23"/>
-      <c r="Z4" s="23"/>
-      <c r="AA4" s="24"/>
-      <c r="AB4" s="27">
+      <c r="V4" s="46"/>
+      <c r="W4" s="46"/>
+      <c r="X4" s="46"/>
+      <c r="Y4" s="46"/>
+      <c r="Z4" s="46"/>
+      <c r="AA4" s="47"/>
+      <c r="AB4" s="45">
         <f>AB5</f>
         <v>45099</v>
       </c>
-      <c r="AC4" s="23"/>
-      <c r="AD4" s="23"/>
-      <c r="AE4" s="23"/>
-      <c r="AF4" s="23"/>
-      <c r="AG4" s="23"/>
-      <c r="AH4" s="24"/>
-      <c r="AI4" s="46"/>
-      <c r="AJ4" s="47"/>
-      <c r="AK4" s="47"/>
-      <c r="AL4" s="47"/>
-      <c r="AM4" s="47"/>
-      <c r="AN4" s="47"/>
-      <c r="AO4" s="48"/>
-      <c r="AP4" s="46"/>
-      <c r="AQ4" s="47"/>
-      <c r="AR4" s="47"/>
-      <c r="AS4" s="47"/>
-      <c r="AT4" s="47"/>
-      <c r="AU4" s="47"/>
-      <c r="AV4" s="48"/>
+      <c r="AC4" s="46"/>
+      <c r="AD4" s="46"/>
+      <c r="AE4" s="46"/>
+      <c r="AF4" s="46"/>
+      <c r="AG4" s="46"/>
+      <c r="AH4" s="47"/>
+      <c r="AI4" s="41"/>
+      <c r="AJ4" s="42"/>
+      <c r="AK4" s="42"/>
+      <c r="AL4" s="42"/>
+      <c r="AM4" s="42"/>
+      <c r="AN4" s="42"/>
+      <c r="AO4" s="43"/>
+      <c r="AP4" s="41"/>
+      <c r="AQ4" s="42"/>
+      <c r="AR4" s="42"/>
+      <c r="AS4" s="42"/>
+      <c r="AT4" s="42"/>
+      <c r="AU4" s="42"/>
+      <c r="AV4" s="43"/>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="18">
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="48">
         <v>45078</v>
       </c>
-      <c r="E5" s="18"/>
+      <c r="E5" s="48"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="29">
+      <c r="G5" s="24">
         <f>E4</f>
         <v>45078</v>
       </c>
-      <c r="H5" s="30">
-        <f t="shared" ref="H5:AK5" si="0">G5+1</f>
+      <c r="H5" s="25">
+        <f t="shared" ref="H5:AH5" si="0">G5+1</f>
         <v>45079</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="25">
         <f t="shared" si="0"/>
         <v>45080</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5" s="25">
         <f t="shared" si="0"/>
         <v>45081</v>
       </c>
-      <c r="K5" s="30">
+      <c r="K5" s="25">
         <f t="shared" si="0"/>
         <v>45082</v>
       </c>
-      <c r="L5" s="30">
+      <c r="L5" s="25">
         <f t="shared" si="0"/>
         <v>45083</v>
       </c>
-      <c r="M5" s="31">
+      <c r="M5" s="26">
         <f t="shared" si="0"/>
         <v>45084</v>
       </c>
-      <c r="N5" s="32">
+      <c r="N5" s="27">
         <f t="shared" si="0"/>
         <v>45085</v>
       </c>
-      <c r="O5" s="30">
+      <c r="O5" s="25">
         <f t="shared" si="0"/>
         <v>45086</v>
       </c>
-      <c r="P5" s="30">
+      <c r="P5" s="25">
         <f t="shared" si="0"/>
         <v>45087</v>
       </c>
-      <c r="Q5" s="30">
+      <c r="Q5" s="25">
         <f t="shared" si="0"/>
         <v>45088</v>
       </c>
-      <c r="R5" s="30">
+      <c r="R5" s="25">
         <f t="shared" si="0"/>
         <v>45089</v>
       </c>
-      <c r="S5" s="30">
+      <c r="S5" s="25">
         <f t="shared" si="0"/>
         <v>45090</v>
       </c>
-      <c r="T5" s="31">
+      <c r="T5" s="26">
         <f t="shared" si="0"/>
         <v>45091</v>
       </c>
-      <c r="U5" s="32">
+      <c r="U5" s="27">
         <f t="shared" si="0"/>
         <v>45092</v>
       </c>
-      <c r="V5" s="30">
+      <c r="V5" s="25">
         <f t="shared" si="0"/>
         <v>45093</v>
       </c>
-      <c r="W5" s="30">
+      <c r="W5" s="25">
         <f t="shared" si="0"/>
         <v>45094</v>
       </c>
-      <c r="X5" s="30">
+      <c r="X5" s="25">
         <f t="shared" si="0"/>
         <v>45095</v>
       </c>
-      <c r="Y5" s="30">
+      <c r="Y5" s="25">
         <f t="shared" si="0"/>
         <v>45096</v>
       </c>
-      <c r="Z5" s="30">
+      <c r="Z5" s="25">
         <f t="shared" si="0"/>
         <v>45097</v>
       </c>
-      <c r="AA5" s="31">
+      <c r="AA5" s="26">
         <f t="shared" si="0"/>
         <v>45098</v>
       </c>
-      <c r="AB5" s="32">
+      <c r="AB5" s="27">
         <f t="shared" si="0"/>
         <v>45099</v>
       </c>
-      <c r="AC5" s="30">
+      <c r="AC5" s="25">
         <f t="shared" si="0"/>
         <v>45100</v>
       </c>
-      <c r="AD5" s="30">
+      <c r="AD5" s="25">
         <f t="shared" si="0"/>
         <v>45101</v>
       </c>
-      <c r="AE5" s="30">
+      <c r="AE5" s="25">
         <f t="shared" si="0"/>
         <v>45102</v>
       </c>
-      <c r="AF5" s="30">
+      <c r="AF5" s="25">
         <f t="shared" si="0"/>
         <v>45103</v>
       </c>
-      <c r="AG5" s="30">
+      <c r="AG5" s="25">
         <f t="shared" si="0"/>
         <v>45104</v>
       </c>
-      <c r="AH5" s="31">
+      <c r="AH5" s="26">
         <f t="shared" si="0"/>
         <v>45105</v>
       </c>
-      <c r="AI5" s="40"/>
-      <c r="AJ5" s="41"/>
-      <c r="AK5" s="41"/>
-      <c r="AL5" s="41"/>
-      <c r="AM5" s="41"/>
-      <c r="AN5" s="41"/>
-      <c r="AO5" s="42"/>
-      <c r="AP5" s="40"/>
-      <c r="AQ5" s="41"/>
-      <c r="AR5" s="41"/>
-      <c r="AS5" s="41"/>
-      <c r="AT5" s="41"/>
-      <c r="AU5" s="41"/>
-      <c r="AV5" s="42"/>
+      <c r="AI5" s="35"/>
+      <c r="AJ5" s="36"/>
+      <c r="AK5" s="36"/>
+      <c r="AL5" s="36"/>
+      <c r="AM5" s="36"/>
+      <c r="AN5" s="36"/>
+      <c r="AO5" s="37"/>
+      <c r="AP5" s="35"/>
+      <c r="AQ5" s="36"/>
+      <c r="AR5" s="36"/>
+      <c r="AS5" s="36"/>
+      <c r="AT5" s="36"/>
+      <c r="AU5" s="36"/>
+      <c r="AV5" s="37"/>
     </row>
     <row r="6" spans="1:48" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1022,132 +1022,132 @@
         <v>13</v>
       </c>
       <c r="F6" s="8"/>
-      <c r="G6" s="28" t="str">
+      <c r="G6" s="23" t="str">
         <f>UPPER(LEFT(TEXT(G5,"ddd"),1))</f>
         <v>J</v>
       </c>
-      <c r="H6" s="25" t="str">
-        <f t="shared" ref="H6:AK6" si="1">UPPER(LEFT(TEXT(H5,"ddd"),1))</f>
+      <c r="H6" s="21" t="str">
+        <f t="shared" ref="H6:AH6" si="1">UPPER(LEFT(TEXT(H5,"ddd"),1))</f>
         <v>V</v>
       </c>
-      <c r="I6" s="25" t="str">
+      <c r="I6" s="21" t="str">
         <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="J6" s="25" t="str">
+      <c r="J6" s="21" t="str">
         <f t="shared" si="1"/>
         <v>D</v>
       </c>
-      <c r="K6" s="25" t="str">
+      <c r="K6" s="21" t="str">
         <f t="shared" si="1"/>
         <v>L</v>
       </c>
-      <c r="L6" s="25" t="str">
+      <c r="L6" s="21" t="str">
         <f t="shared" si="1"/>
         <v>M</v>
       </c>
-      <c r="M6" s="26" t="str">
+      <c r="M6" s="22" t="str">
         <f t="shared" si="1"/>
         <v>M</v>
       </c>
-      <c r="N6" s="28" t="str">
+      <c r="N6" s="23" t="str">
         <f t="shared" si="1"/>
         <v>J</v>
       </c>
-      <c r="O6" s="25" t="str">
+      <c r="O6" s="21" t="str">
         <f t="shared" si="1"/>
         <v>V</v>
       </c>
-      <c r="P6" s="25" t="str">
+      <c r="P6" s="21" t="str">
         <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="Q6" s="25" t="str">
+      <c r="Q6" s="21" t="str">
         <f t="shared" si="1"/>
         <v>D</v>
       </c>
-      <c r="R6" s="25" t="str">
+      <c r="R6" s="21" t="str">
         <f t="shared" si="1"/>
         <v>L</v>
       </c>
-      <c r="S6" s="25" t="str">
+      <c r="S6" s="21" t="str">
         <f t="shared" si="1"/>
         <v>M</v>
       </c>
-      <c r="T6" s="26" t="str">
+      <c r="T6" s="22" t="str">
         <f t="shared" si="1"/>
         <v>M</v>
       </c>
-      <c r="U6" s="28" t="str">
+      <c r="U6" s="23" t="str">
         <f t="shared" si="1"/>
         <v>J</v>
       </c>
-      <c r="V6" s="25" t="str">
+      <c r="V6" s="21" t="str">
         <f t="shared" si="1"/>
         <v>V</v>
       </c>
-      <c r="W6" s="25" t="str">
+      <c r="W6" s="21" t="str">
         <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="X6" s="25" t="str">
+      <c r="X6" s="21" t="str">
         <f t="shared" si="1"/>
         <v>D</v>
       </c>
-      <c r="Y6" s="25" t="str">
+      <c r="Y6" s="21" t="str">
         <f t="shared" si="1"/>
         <v>L</v>
       </c>
-      <c r="Z6" s="25" t="str">
+      <c r="Z6" s="21" t="str">
         <f t="shared" si="1"/>
         <v>M</v>
       </c>
-      <c r="AA6" s="26" t="str">
+      <c r="AA6" s="22" t="str">
         <f t="shared" si="1"/>
         <v>M</v>
       </c>
-      <c r="AB6" s="28" t="str">
+      <c r="AB6" s="23" t="str">
         <f t="shared" si="1"/>
         <v>J</v>
       </c>
-      <c r="AC6" s="25" t="str">
+      <c r="AC6" s="21" t="str">
         <f t="shared" si="1"/>
         <v>V</v>
       </c>
-      <c r="AD6" s="25" t="str">
+      <c r="AD6" s="21" t="str">
         <f t="shared" si="1"/>
         <v>S</v>
       </c>
-      <c r="AE6" s="25" t="str">
+      <c r="AE6" s="21" t="str">
         <f t="shared" si="1"/>
         <v>D</v>
       </c>
-      <c r="AF6" s="25" t="str">
+      <c r="AF6" s="21" t="str">
         <f t="shared" si="1"/>
         <v>L</v>
       </c>
-      <c r="AG6" s="25" t="str">
+      <c r="AG6" s="21" t="str">
         <f t="shared" si="1"/>
         <v>M</v>
       </c>
-      <c r="AH6" s="26" t="str">
+      <c r="AH6" s="22" t="str">
         <f t="shared" si="1"/>
         <v>M</v>
       </c>
-      <c r="AI6" s="43"/>
-      <c r="AJ6" s="44"/>
-      <c r="AK6" s="44"/>
-      <c r="AL6" s="44"/>
-      <c r="AM6" s="44"/>
-      <c r="AN6" s="44"/>
-      <c r="AO6" s="45"/>
-      <c r="AP6" s="43"/>
-      <c r="AQ6" s="44"/>
-      <c r="AR6" s="44"/>
-      <c r="AS6" s="44"/>
-      <c r="AT6" s="44"/>
-      <c r="AU6" s="44"/>
-      <c r="AV6" s="45"/>
+      <c r="AI6" s="38"/>
+      <c r="AJ6" s="39"/>
+      <c r="AK6" s="39"/>
+      <c r="AL6" s="39"/>
+      <c r="AM6" s="39"/>
+      <c r="AN6" s="39"/>
+      <c r="AO6" s="40"/>
+      <c r="AP6" s="38"/>
+      <c r="AQ6" s="39"/>
+      <c r="AR6" s="39"/>
+      <c r="AS6" s="39"/>
+      <c r="AT6" s="39"/>
+      <c r="AU6" s="39"/>
+      <c r="AV6" s="40"/>
     </row>
     <row r="7" spans="1:48" s="13" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
@@ -1159,31 +1159,31 @@
       <c r="C7" s="9">
         <v>1</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="20">
         <v>45082</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="20">
         <v>45096</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="34"/>
-      <c r="Q7" s="34"/>
-      <c r="R7" s="34"/>
-      <c r="S7" s="34"/>
-      <c r="T7" s="34"/>
-      <c r="U7" s="34"/>
-      <c r="V7" s="34"/>
-      <c r="W7" s="34"/>
-      <c r="X7" s="34"/>
-      <c r="Y7" s="34"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="29"/>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="29"/>
       <c r="Z7" s="14"/>
       <c r="AA7" s="14"/>
       <c r="AB7" s="14"/>
@@ -1218,31 +1218,31 @@
       <c r="C8" s="9">
         <v>1</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="20">
         <v>45082</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="20">
         <v>45096</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="33"/>
-      <c r="R8" s="33"/>
-      <c r="S8" s="33"/>
-      <c r="T8" s="33"/>
-      <c r="U8" s="33"/>
-      <c r="V8" s="33"/>
-      <c r="W8" s="33"/>
-      <c r="X8" s="33"/>
-      <c r="Y8" s="33"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="28"/>
+      <c r="U8" s="28"/>
+      <c r="V8" s="28"/>
+      <c r="W8" s="28"/>
+      <c r="X8" s="28"/>
+      <c r="Y8" s="28"/>
       <c r="Z8" s="14"/>
       <c r="AA8" s="14"/>
       <c r="AB8" s="14"/>
@@ -1277,31 +1277,31 @@
       <c r="C9" s="9">
         <v>1</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="20">
         <v>45082</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="20">
         <v>45096</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
-      <c r="O9" s="49"/>
-      <c r="P9" s="49"/>
-      <c r="Q9" s="33"/>
-      <c r="R9" s="33"/>
-      <c r="S9" s="33"/>
-      <c r="T9" s="33"/>
-      <c r="U9" s="33"/>
-      <c r="V9" s="33"/>
-      <c r="W9" s="33"/>
-      <c r="X9" s="33"/>
-      <c r="Y9" s="33"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="44"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="28"/>
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="28"/>
+      <c r="X9" s="28"/>
+      <c r="Y9" s="28"/>
       <c r="Z9" s="14"/>
       <c r="AA9" s="14"/>
       <c r="AB9" s="14"/>
@@ -1336,23 +1336,23 @@
       <c r="C10" s="9">
         <v>1</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="20">
         <v>45097</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="20">
         <v>45107</v>
       </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="34"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="29"/>
       <c r="R10" s="14"/>
       <c r="S10" s="14"/>
       <c r="T10" s="14"/>
@@ -1361,17 +1361,17 @@
       <c r="W10" s="14"/>
       <c r="X10" s="14"/>
       <c r="Y10" s="14"/>
-      <c r="Z10" s="34"/>
-      <c r="AA10" s="34"/>
-      <c r="AB10" s="34"/>
-      <c r="AC10" s="34"/>
-      <c r="AD10" s="34"/>
-      <c r="AE10" s="34"/>
-      <c r="AF10" s="34"/>
-      <c r="AG10" s="34"/>
-      <c r="AH10" s="34"/>
-      <c r="AI10" s="34"/>
-      <c r="AJ10" s="34"/>
+      <c r="Z10" s="29"/>
+      <c r="AA10" s="29"/>
+      <c r="AB10" s="29"/>
+      <c r="AC10" s="29"/>
+      <c r="AD10" s="29"/>
+      <c r="AE10" s="29"/>
+      <c r="AF10" s="29"/>
+      <c r="AG10" s="29"/>
+      <c r="AH10" s="29"/>
+      <c r="AI10" s="29"/>
+      <c r="AJ10" s="29"/>
       <c r="AK10" s="14"/>
       <c r="AL10" s="14"/>
       <c r="AM10" s="14"/>
@@ -1395,23 +1395,23 @@
       <c r="C11" s="9">
         <v>1</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="20">
         <v>45097</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="20">
         <v>45107</v>
       </c>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
-      <c r="Q11" s="33"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
       <c r="R11" s="14"/>
       <c r="S11" s="14"/>
       <c r="T11" s="14"/>
@@ -1420,17 +1420,17 @@
       <c r="W11" s="14"/>
       <c r="X11" s="14"/>
       <c r="Y11" s="14"/>
-      <c r="Z11" s="33"/>
-      <c r="AA11" s="33"/>
-      <c r="AB11" s="33"/>
-      <c r="AC11" s="33"/>
-      <c r="AD11" s="33"/>
-      <c r="AE11" s="33"/>
-      <c r="AF11" s="33"/>
-      <c r="AG11" s="33"/>
-      <c r="AH11" s="33"/>
-      <c r="AI11" s="33"/>
-      <c r="AJ11" s="33"/>
+      <c r="Z11" s="28"/>
+      <c r="AA11" s="28"/>
+      <c r="AB11" s="28"/>
+      <c r="AC11" s="28"/>
+      <c r="AD11" s="28"/>
+      <c r="AE11" s="28"/>
+      <c r="AF11" s="28"/>
+      <c r="AG11" s="28"/>
+      <c r="AH11" s="28"/>
+      <c r="AI11" s="28"/>
+      <c r="AJ11" s="28"/>
       <c r="AK11" s="14"/>
       <c r="AL11" s="14"/>
       <c r="AM11" s="14"/>
@@ -1454,54 +1454,54 @@
       <c r="C12" s="9">
         <v>1</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="20">
         <v>45121</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="20">
         <v>45142</v>
       </c>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="34"/>
-      <c r="P12" s="34"/>
-      <c r="Q12" s="34"/>
-      <c r="R12" s="34"/>
-      <c r="S12" s="34"/>
-      <c r="T12" s="34"/>
-      <c r="U12" s="34"/>
-      <c r="V12" s="34"/>
-      <c r="W12" s="34"/>
-      <c r="X12" s="34"/>
-      <c r="Y12" s="34"/>
-      <c r="Z12" s="34"/>
-      <c r="AA12" s="34"/>
-      <c r="AB12" s="34"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="29"/>
+      <c r="T12" s="29"/>
+      <c r="U12" s="29"/>
+      <c r="V12" s="29"/>
+      <c r="W12" s="29"/>
+      <c r="X12" s="29"/>
+      <c r="Y12" s="29"/>
+      <c r="Z12" s="29"/>
+      <c r="AA12" s="29"/>
+      <c r="AB12" s="29"/>
       <c r="AC12" s="14"/>
       <c r="AD12" s="14"/>
-      <c r="AE12" s="34"/>
-      <c r="AF12" s="34"/>
-      <c r="AG12" s="34"/>
-      <c r="AH12" s="34"/>
-      <c r="AI12" s="34"/>
-      <c r="AJ12" s="34"/>
-      <c r="AK12" s="34"/>
-      <c r="AL12" s="34"/>
-      <c r="AM12" s="34"/>
-      <c r="AN12" s="34"/>
-      <c r="AO12" s="34"/>
-      <c r="AP12" s="34"/>
-      <c r="AQ12" s="34"/>
-      <c r="AR12" s="34"/>
-      <c r="AS12" s="34"/>
-      <c r="AT12" s="34"/>
-      <c r="AU12" s="34"/>
-      <c r="AV12" s="34"/>
+      <c r="AE12" s="29"/>
+      <c r="AF12" s="29"/>
+      <c r="AG12" s="29"/>
+      <c r="AH12" s="29"/>
+      <c r="AI12" s="29"/>
+      <c r="AJ12" s="29"/>
+      <c r="AK12" s="29"/>
+      <c r="AL12" s="29"/>
+      <c r="AM12" s="29"/>
+      <c r="AN12" s="29"/>
+      <c r="AO12" s="29"/>
+      <c r="AP12" s="29"/>
+      <c r="AQ12" s="29"/>
+      <c r="AR12" s="29"/>
+      <c r="AS12" s="29"/>
+      <c r="AT12" s="29"/>
+      <c r="AU12" s="29"/>
+      <c r="AV12" s="29"/>
     </row>
     <row r="13" spans="1:48" s="13" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
@@ -1513,20 +1513,20 @@
       <c r="C13" s="9">
         <v>1</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="20">
         <v>45121</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="20">
         <v>45128</v>
       </c>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
       <c r="O13" s="14"/>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
@@ -1543,14 +1543,14 @@
       <c r="AB13" s="14"/>
       <c r="AC13" s="14"/>
       <c r="AD13" s="14"/>
-      <c r="AE13" s="33"/>
-      <c r="AF13" s="33"/>
-      <c r="AG13" s="33"/>
-      <c r="AH13" s="33"/>
-      <c r="AI13" s="33"/>
-      <c r="AJ13" s="33"/>
-      <c r="AK13" s="33"/>
-      <c r="AL13" s="33"/>
+      <c r="AE13" s="28"/>
+      <c r="AF13" s="28"/>
+      <c r="AG13" s="28"/>
+      <c r="AH13" s="28"/>
+      <c r="AI13" s="28"/>
+      <c r="AJ13" s="28"/>
+      <c r="AK13" s="28"/>
+      <c r="AL13" s="28"/>
       <c r="AM13" s="14"/>
       <c r="AN13" s="14"/>
       <c r="AO13" s="14"/>
@@ -1572,29 +1572,29 @@
       <c r="C14" s="9">
         <v>1</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="20">
         <v>45153</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="20">
         <v>45169</v>
       </c>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="34"/>
-      <c r="P14" s="34"/>
-      <c r="Q14" s="34"/>
-      <c r="R14" s="34"/>
-      <c r="S14" s="34"/>
-      <c r="T14" s="34"/>
-      <c r="U14" s="34"/>
-      <c r="V14" s="34"/>
-      <c r="W14" s="34"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="29"/>
+      <c r="T14" s="29"/>
+      <c r="U14" s="29"/>
+      <c r="V14" s="29"/>
+      <c r="W14" s="29"/>
       <c r="X14" s="14"/>
       <c r="Y14" s="14"/>
       <c r="Z14" s="14"/>
@@ -1631,29 +1631,29 @@
       <c r="C15" s="9">
         <v>1</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="20">
         <v>45153</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="20">
         <v>45169</v>
       </c>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="33"/>
-      <c r="O15" s="33"/>
-      <c r="P15" s="33"/>
-      <c r="Q15" s="33"/>
-      <c r="R15" s="33"/>
-      <c r="S15" s="33"/>
-      <c r="T15" s="33"/>
-      <c r="U15" s="33"/>
-      <c r="V15" s="33"/>
-      <c r="W15" s="33"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="28"/>
       <c r="X15" s="14"/>
       <c r="Y15" s="14"/>
       <c r="Z15" s="14"/>
@@ -1690,10 +1690,10 @@
       <c r="C16" s="9">
         <v>1</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="20">
         <v>45173</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="20">
         <v>45180</v>
       </c>
       <c r="G16" s="14"/>
@@ -1716,14 +1716,14 @@
       <c r="X16" s="14"/>
       <c r="Y16" s="14"/>
       <c r="Z16" s="14"/>
-      <c r="AA16" s="34"/>
-      <c r="AB16" s="34"/>
-      <c r="AC16" s="34"/>
-      <c r="AD16" s="34"/>
-      <c r="AE16" s="34"/>
-      <c r="AF16" s="34"/>
-      <c r="AG16" s="34"/>
-      <c r="AH16" s="34"/>
+      <c r="AA16" s="29"/>
+      <c r="AB16" s="29"/>
+      <c r="AC16" s="29"/>
+      <c r="AD16" s="29"/>
+      <c r="AE16" s="29"/>
+      <c r="AF16" s="29"/>
+      <c r="AG16" s="29"/>
+      <c r="AH16" s="29"/>
       <c r="AI16" s="14"/>
       <c r="AJ16" s="14"/>
       <c r="AK16" s="14"/>
@@ -1755,44 +1755,44 @@
       <c r="E17" s="6">
         <v>45261</v>
       </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="20"/>
-      <c r="R17" s="20"/>
-      <c r="S17" s="20"/>
-      <c r="T17" s="20"/>
-      <c r="U17" s="20"/>
-      <c r="V17" s="20"/>
-      <c r="W17" s="20"/>
-      <c r="X17" s="20"/>
-      <c r="Y17" s="20"/>
-      <c r="Z17" s="20"/>
-      <c r="AA17" s="20"/>
-      <c r="AB17" s="20"/>
-      <c r="AC17" s="20"/>
-      <c r="AD17" s="20"/>
-      <c r="AE17" s="20"/>
-      <c r="AF17" s="20"/>
-      <c r="AG17" s="20"/>
-      <c r="AH17" s="20"/>
-      <c r="AI17" s="20"/>
-      <c r="AJ17" s="20"/>
-      <c r="AK17" s="20"/>
-      <c r="AL17" s="20"/>
-      <c r="AM17" s="20"/>
-      <c r="AN17" s="20"/>
-      <c r="AO17" s="20"/>
-      <c r="AP17" s="20"/>
-      <c r="AQ17" s="20"/>
-      <c r="AR17" s="20"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18"/>
+      <c r="S17" s="18"/>
+      <c r="T17" s="18"/>
+      <c r="U17" s="18"/>
+      <c r="V17" s="18"/>
+      <c r="W17" s="18"/>
+      <c r="X17" s="18"/>
+      <c r="Y17" s="18"/>
+      <c r="Z17" s="18"/>
+      <c r="AA17" s="18"/>
+      <c r="AB17" s="18"/>
+      <c r="AC17" s="18"/>
+      <c r="AD17" s="18"/>
+      <c r="AE17" s="18"/>
+      <c r="AF17" s="18"/>
+      <c r="AG17" s="18"/>
+      <c r="AH17" s="18"/>
+      <c r="AI17" s="18"/>
+      <c r="AJ17" s="18"/>
+      <c r="AK17" s="18"/>
+      <c r="AL17" s="18"/>
+      <c r="AM17" s="18"/>
+      <c r="AN17" s="18"/>
+      <c r="AO17" s="18"/>
+      <c r="AP17" s="18"/>
+      <c r="AQ17" s="18"/>
+      <c r="AR17" s="18"/>
       <c r="AS17" s="11"/>
       <c r="AT17" s="11"/>
       <c r="AU17" s="11"/>
@@ -1877,7 +1877,7 @@
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
-      <c r="K19" s="21"/>
+      <c r="K19" s="19"/>
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
       <c r="N19" s="12"/>
@@ -2101,7 +2101,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="9">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="D23" s="6">
         <v>45255</v>
@@ -2109,9 +2109,9 @@
       <c r="E23" s="6">
         <v>45261</v>
       </c>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
       <c r="J23" s="11"/>
       <c r="K23" s="11"/>
       <c r="L23" s="11"/>
@@ -2164,13 +2164,13 @@
       <c r="E24" s="6">
         <v>45267</v>
       </c>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37"/>
-      <c r="O24" s="37"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="32"/>
     </row>
     <row r="25" spans="1:48" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
@@ -2188,15 +2188,15 @@
       <c r="E25" s="6">
         <v>45267</v>
       </c>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="38"/>
-      <c r="N25" s="38"/>
-      <c r="O25" s="38"/>
-    </row>
-    <row r="26" spans="1:48" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33"/>
+    </row>
+    <row r="26" spans="1:48" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>20</v>
       </c>
@@ -2212,13 +2212,13 @@
       <c r="E26" s="6">
         <v>45267</v>
       </c>
-      <c r="I26" s="38"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="38"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="38"/>
-      <c r="O26" s="38"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="33"/>
+      <c r="O26" s="33"/>
     </row>
     <row r="27" spans="1:48" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
@@ -2236,13 +2236,13 @@
       <c r="E27" s="6">
         <v>45267</v>
       </c>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="38"/>
-      <c r="N27" s="38"/>
-      <c r="O27" s="38"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="33"/>
+      <c r="O27" s="33"/>
     </row>
     <row r="28" spans="1:48" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
@@ -2260,23 +2260,23 @@
       <c r="E28" s="6">
         <v>45267</v>
       </c>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="38"/>
-      <c r="M28" s="38"/>
-      <c r="N28" s="38"/>
-      <c r="O28" s="38"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+      <c r="O28" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A5:C5"/>
     <mergeCell ref="AB4:AH4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="G4:M4"/>
     <mergeCell ref="N4:T4"/>
     <mergeCell ref="U4:AA4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:C28">
     <cfRule type="dataBar" priority="12">

</xml_diff>